<commit_message>
work on filter table
</commit_message>
<xml_diff>
--- a/PAHL Fall 2022 Schedule2.xlsx
+++ b/PAHL Fall 2022 Schedule2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredy\Desktop\dev\Ironhack\Module 2\Hockey App\Hockey-App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC3DF79-2527-49A0-BF9A-1D90758A4CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E28DC2-A179-4D4A-A3F1-9C6A17110FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DBE2A0E6-F181-415A-81E2-ADF6E6432545}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DBE2A0E6-F181-415A-81E2-ADF6E6432545}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2431" uniqueCount="123">
   <si>
     <t>Monday</t>
   </si>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937FCDD3-DE25-4DF3-8880-4A4DD64D582B}">
   <dimension ref="A1:K476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D73" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -11868,10 +11868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960EB9DB-C53C-4D1B-A6AC-8AE2CE148D23}">
-  <dimension ref="A1:D780"/>
+  <dimension ref="A1:J780"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11879,476 +11879,832 @@
     <col min="1" max="1" width="27.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" style="2"/>
+    <col min="7" max="7" width="29" style="2" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>44830</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="5">
+        <v>44832</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="7">
+        <v>44833</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="5">
+        <v>44836</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="5">
+        <v>44837</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="5">
+        <v>44838</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="5">
+        <v>44839</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G9" s="5">
+        <v>44840</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D10"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G10" s="5">
+        <v>44843</v>
+      </c>
+      <c r="J10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D11"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G11" s="5">
+        <v>44844</v>
+      </c>
+      <c r="J11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D12"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G12" s="5">
+        <v>44845</v>
+      </c>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D13"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G13" s="5">
+        <v>44846</v>
+      </c>
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D14"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G14" s="5">
+        <v>44847</v>
+      </c>
+      <c r="J14"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D15"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G15" s="5">
+        <v>44850</v>
+      </c>
+      <c r="J15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D16"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G16" s="7">
+        <v>44851</v>
+      </c>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>111</v>
       </c>
       <c r="D17"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G17" s="5">
+        <v>44852</v>
+      </c>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D18"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G18" s="5">
+        <v>44854</v>
+      </c>
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>95</v>
       </c>
       <c r="D19"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G19" s="5">
+        <v>44857</v>
+      </c>
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D20"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G20" s="7">
+        <v>44858</v>
+      </c>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D21"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G21" s="5">
+        <v>44859</v>
+      </c>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>66</v>
       </c>
       <c r="D22"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G22" s="5">
+        <v>44860</v>
+      </c>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D23"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G23" s="5">
+        <v>44861</v>
+      </c>
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D24"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G24" s="5">
+        <v>44864</v>
+      </c>
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>98</v>
       </c>
       <c r="D25"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G25" s="5">
+        <v>44865</v>
+      </c>
+      <c r="J25"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D26"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G26" s="7">
+        <v>44866</v>
+      </c>
+      <c r="J26"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D27"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G27" s="7">
+        <v>44867</v>
+      </c>
+      <c r="J27"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D28"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G28" s="5">
+        <v>44868</v>
+      </c>
+      <c r="J28"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D29"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G29" s="5">
+        <v>44871</v>
+      </c>
+      <c r="J29"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D30"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G30" s="5">
+        <v>44872</v>
+      </c>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>101</v>
       </c>
       <c r="D31"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G31" s="5">
+        <v>44873</v>
+      </c>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D32"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G32" s="7">
+        <v>44874</v>
+      </c>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D33"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G33" s="7">
+        <v>44875</v>
+      </c>
+      <c r="J33"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D34"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G34" s="5">
+        <v>44878</v>
+      </c>
+      <c r="J34"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D35"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G35" s="5">
+        <v>44879</v>
+      </c>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D36"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G36" s="5">
+        <v>44880</v>
+      </c>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D37"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G37" s="5">
+        <v>44881</v>
+      </c>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D38"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G38" s="5">
+        <v>44882</v>
+      </c>
+      <c r="J38"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D39"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G39" s="5">
+        <v>44885</v>
+      </c>
+      <c r="J39"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D40"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G40" s="5">
+        <v>44886</v>
+      </c>
+      <c r="J40"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D41"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G41" s="5">
+        <v>44887</v>
+      </c>
+      <c r="J41"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D42"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G42" s="5">
+        <v>44888</v>
+      </c>
+      <c r="J42"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D43"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G43" s="5">
+        <v>44893</v>
+      </c>
+      <c r="J43"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D44"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G44" s="7">
+        <v>44894</v>
+      </c>
+      <c r="J44"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>70</v>
       </c>
       <c r="D45"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G45" s="7">
+        <v>44895</v>
+      </c>
+      <c r="J45"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D46"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G46" s="5">
+        <v>44896</v>
+      </c>
+      <c r="J46"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D47"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G47" s="5">
+        <v>44899</v>
+      </c>
+      <c r="J47"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D48"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G48" s="5">
+        <v>44900</v>
+      </c>
+      <c r="J48"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D49"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G49" s="5">
+        <v>44901</v>
+      </c>
+      <c r="J49"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>113</v>
       </c>
       <c r="D50"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G50" s="5">
+        <v>44902</v>
+      </c>
+      <c r="J50"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D51"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G51" s="7">
+        <v>44903</v>
+      </c>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D52"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G52" s="7">
+        <v>44906</v>
+      </c>
+      <c r="J52"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D53"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G53" s="5">
+        <v>44907</v>
+      </c>
+      <c r="J53"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D54"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G54" s="5">
+        <v>44908</v>
+      </c>
+      <c r="J54"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D55"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G55" s="7">
+        <v>44909</v>
+      </c>
+      <c r="J55"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>102</v>
       </c>
       <c r="D56"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G56" s="5">
+        <v>44910</v>
+      </c>
+      <c r="J56"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D57"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G57" s="7">
+        <v>44913</v>
+      </c>
+      <c r="J57"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D58"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G58" s="5">
+        <v>44914</v>
+      </c>
+      <c r="J58"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D59"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G59" s="5">
+        <v>44915</v>
+      </c>
+      <c r="J59"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D60"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G60" s="5">
+        <v>44916</v>
+      </c>
+      <c r="J60"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D61"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G61" s="5">
+        <v>44917</v>
+      </c>
+      <c r="J61"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D62"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G62" s="5">
+        <v>44928</v>
+      </c>
+      <c r="J62"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D63"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G63" s="7">
+        <v>44929</v>
+      </c>
+      <c r="J63"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D64"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G64" s="7">
+        <v>44930</v>
+      </c>
+      <c r="J64"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D65"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G65" s="5">
+        <v>44931</v>
+      </c>
+      <c r="J65"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>80</v>
       </c>
       <c r="D66"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G66" s="5">
+        <v>44934</v>
+      </c>
+      <c r="J66"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67"/>
       <c r="D67"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G67" s="7">
+        <v>44935</v>
+      </c>
+      <c r="J67"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="D68"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G68" s="7">
+        <v>44936</v>
+      </c>
+      <c r="J68"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="D69"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G69" s="5">
+        <v>44937</v>
+      </c>
+      <c r="J69"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="D70"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G70" s="7">
+        <v>44938</v>
+      </c>
+      <c r="J70"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="D71"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G71" s="5">
+        <v>44941</v>
+      </c>
+      <c r="J71"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="D72"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G72" s="5">
+        <v>44942</v>
+      </c>
+      <c r="J72"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="D73"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G73" s="5">
+        <v>44943</v>
+      </c>
+      <c r="J73"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74"/>
       <c r="D74"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G74" s="5">
+        <v>44944</v>
+      </c>
+      <c r="J74"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75"/>
       <c r="D75"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G75" s="7">
+        <v>44945</v>
+      </c>
+      <c r="J75"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76"/>
       <c r="D76"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G76" s="7">
+        <v>44948</v>
+      </c>
+      <c r="J76"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77"/>
       <c r="D77"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G77" s="7">
+        <v>44950</v>
+      </c>
+      <c r="J77"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78"/>
       <c r="D78"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G78" s="7">
+        <v>44951</v>
+      </c>
+      <c r="J78"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79"/>
       <c r="D79"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G79" s="5">
+        <v>44955</v>
+      </c>
+      <c r="J79"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="D80"/>
-    </row>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="G80" s="5">
+        <v>44962</v>
+      </c>
+      <c r="J80"/>
+    </row>
+    <row r="81" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G81" s="5"/>
+    </row>
+    <row r="82" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="7:7" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="97" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="98" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="99" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -13183,52 +13539,76 @@
     <row r="766" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="767" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="768" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="769" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="769" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A769"/>
       <c r="D769"/>
-    </row>
-    <row r="770" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G769"/>
+      <c r="J769"/>
+    </row>
+    <row r="770" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A770"/>
       <c r="D770"/>
-    </row>
-    <row r="771" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G770"/>
+      <c r="J770"/>
+    </row>
+    <row r="771" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A771"/>
       <c r="D771"/>
-    </row>
-    <row r="772" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G771"/>
+      <c r="J771"/>
+    </row>
+    <row r="772" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A772"/>
       <c r="D772"/>
-    </row>
-    <row r="773" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G772"/>
+      <c r="J772"/>
+    </row>
+    <row r="773" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A773"/>
       <c r="D773"/>
-    </row>
-    <row r="774" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G773"/>
+      <c r="J773"/>
+    </row>
+    <row r="774" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A774"/>
       <c r="D774"/>
-    </row>
-    <row r="775" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G774"/>
+      <c r="J774"/>
+    </row>
+    <row r="775" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A775"/>
       <c r="D775"/>
-    </row>
-    <row r="776" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G775"/>
+      <c r="J775"/>
+    </row>
+    <row r="776" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A776"/>
       <c r="D776"/>
-    </row>
-    <row r="777" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G776"/>
+      <c r="J776"/>
+    </row>
+    <row r="777" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A777"/>
       <c r="D777"/>
-    </row>
-    <row r="778" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G777"/>
+      <c r="J777"/>
+    </row>
+    <row r="778" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A778"/>
       <c r="D778"/>
-    </row>
-    <row r="779" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G778"/>
+      <c r="J778"/>
+    </row>
+    <row r="779" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A779"/>
       <c r="D779"/>
-    </row>
-    <row r="780" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G779"/>
+      <c r="J779"/>
+    </row>
+    <row r="780" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D780"/>
+      <c r="G780"/>
+      <c r="J780"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:D779">

</xml_diff>